<commit_message>
Added lor documents for lw
</commit_message>
<xml_diff>
--- a/documents/misc/lor_linh.xlsx
+++ b/documents/misc/lor_linh.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\12-Webpage\cesarlgm.github.io\documents\other\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thecs\Dropbox\1_boston_university\12-Webpage\cesarlgm.github.io\documents\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CA13F4C-507F-418D-BE25-AE4A7D37F4B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78100E0-998A-4B8E-9CD3-A7D767777514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{638C7514-6DD7-43EC-9471-1A63549FF85C}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{638C7514-6DD7-43EC-9471-1A63549FF85C}"/>
   </bookViews>
   <sheets>
     <sheet name="LINH" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>LINH</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>https://cesarlgm.github.io/documents/profile/teaching_statement_cesarlgm.pdf</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>https://cesarlgm.github.io/documents/idn_secondary_expansion.pdf</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +243,21 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -274,16 +295,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -299,7 +317,21 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -307,18 +339,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{1AD1329D-C7AF-459D-800C-A66141BCCC59}"/>
   </cellStyles>
@@ -655,268 +681,268 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.81640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="21.54296875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="46" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="13.81640625" style="3"/>
+    <col min="1" max="2" width="21.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.36328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="46" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="13.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="8" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="8" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="8" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="2"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2"/>
-      <c r="B9" s="8" t="s">
+      <c r="A9" s="9"/>
+      <c r="B9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="2"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="8" t="s">
+      <c r="A10" s="9"/>
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="10">
+      <c r="C10" s="14">
         <v>45092</v>
       </c>
-      <c r="D10" s="2"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="9"/>
+      <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D11" s="2"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="9"/>
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="9" t="s">
+      <c r="C14" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="13" t="s">
+      <c r="A17" s="9"/>
+      <c r="B17" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="2"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="9"/>
+      <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="15"/>
+      <c r="D20" s="12"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="8" t="s">
+      <c r="A21" s="9"/>
+      <c r="B21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="11"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C22" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="15"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="8" t="s">
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C23" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D22" s="15"/>
-    </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="8" t="s">
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="15"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
+  <mergeCells count="21">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A5:A11"/>
@@ -927,12 +953,24 @@
     <mergeCell ref="C9:D9"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A19:A24"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C24:D24"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="C20" r:id="rId1" xr:uid="{0E2D2FDB-A077-4CAA-9EC3-3EB30655C5B0}"/>
-    <hyperlink ref="C21" r:id="rId2" xr:uid="{49BD8D83-6178-44DA-A906-94F6284BAD4D}"/>
-    <hyperlink ref="C22" r:id="rId3" xr:uid="{436C7359-BD13-4327-84FB-BAE220C905ED}"/>
-    <hyperlink ref="C23" r:id="rId4" xr:uid="{588E56D1-DA9E-487B-B956-0868F9BF1232}"/>
+    <hyperlink ref="C22" r:id="rId2" xr:uid="{49BD8D83-6178-44DA-A906-94F6284BAD4D}"/>
+    <hyperlink ref="C23" r:id="rId3" xr:uid="{436C7359-BD13-4327-84FB-BAE220C905ED}"/>
+    <hyperlink ref="C24" r:id="rId4" xr:uid="{588E56D1-DA9E-487B-B956-0868F9BF1232}"/>
+    <hyperlink ref="C21" r:id="rId5" xr:uid="{7EAB8277-69B4-47B0-BC4C-13D80252D68B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>